<commit_message>
Update: Threat Alert Report - 2026-01-07 16:45
</commit_message>
<xml_diff>
--- a/excel_routes/route_JED_ATZ_threats.xlsx
+++ b/excel_routes/route_JED_ATZ_threats.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>18-JAN-26</t>
+          <t>10-JAN-26</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>SM-492</t>
+          <t>SM-454</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Saudia SV-335</t>
+          <t>EgyptAir MS-8224</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>533</v>
+        <v>747</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>526</v>
+        <v>706</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>46</v>
@@ -573,7 +573,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>29-JAN-26</t>
+          <t>10-JAN-26</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -583,17 +583,17 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>EgyptAir MS-644</t>
+          <t>EgyptAir MS-8224</t>
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>586</v>
+        <v>747</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>586</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>46</v>
@@ -618,27 +618,27 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>29-JAN-26</t>
+          <t>10-JAN-26</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>SM-456</t>
+          <t>SM-492</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>EgyptAir MS-666</t>
+          <t>EgyptAir MS-8224</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>586</v>
+        <v>747</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>586</v>
+        <v>646</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>46</v>
@@ -663,27 +663,27 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>29-JAN-26</t>
+          <t>16-JAN-26</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>SM-456</t>
+          <t>SM-492</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>EgyptAir MS-662</t>
+          <t>Saudia SV-335</t>
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>586</v>
+        <v>461</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>586</v>
+        <v>436</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>46</v>
@@ -708,12 +708,12 @@
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>29-JAN-26</t>
+          <t>26-JAN-26</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>SM-456</t>
+          <t>SM-492</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
@@ -722,13 +722,13 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>586</v>
+        <v>476</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>586</v>
+        <v>471</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>46</v>
@@ -745,6 +745,96 @@
         </is>
       </c>
       <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>SAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>29-JAN-26</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>SM-456</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>EgyptAir MS-666</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>586</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>586</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>-16</v>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>LOW THREAT</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>SAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>29-JAN-26</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>SM-456</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>EgyptAir MS-662</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>586</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>586</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>-16</v>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>LOW THREAT</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="inlineStr">
         <is>
           <t>SAR</t>
         </is>

</xml_diff>